<commit_message>
Incluindo a pasta testeUtilidades
</commit_message>
<xml_diff>
--- a/Openpyxl/testando.xlsx
+++ b/Openpyxl/testando.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:B5"/>
+  <dimension ref="B1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,31 +421,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" t="inlineStr">
+    <row r="1">
+      <c r="B1" t="inlineStr">
         <is>
-          <t>GERA Energia</t>
+          <t>Informação1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>GERA Energia</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>GERA Soluções</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GERA Energia</t>
+          <t>Informação3</t>
         </is>
       </c>
     </row>

</xml_diff>